<commit_message>
am modificat fisierul excel
</commit_message>
<xml_diff>
--- a/lab1.xlsx
+++ b/lab1.xlsx
@@ -13,6 +13,14 @@
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>5+3+4=12</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -343,23 +351,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>2</v>
-      </c>
-      <c r="B1">
-        <v>3</v>
-      </c>
-      <c r="C1">
-        <v>4</v>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>